<commit_message>
feat: create tables for user story map follow
</commit_message>
<xml_diff>
--- a/user-story-mapping.xlsx
+++ b/user-story-mapping.xlsx
@@ -1,26 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridel\Documents\Programación_101\MakeItReal\Proyectos\quick_call\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E55956-9FB2-4310-AE2D-4F4D7D9CA981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+  <si>
+    <t>Control de épicas - Quick Call</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Epica</t>
+  </si>
+  <si>
+    <t>Cantidad de HU</t>
+  </si>
+  <si>
+    <t>Profesional</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +69,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,13 +109,368 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +481,122 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3474720</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6204CE6-FFFA-40D3-B02F-034D442C68B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="601980" y="198120"/>
+          <a:ext cx="10447020" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:latin typeface="Open sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Open sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Open sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>El propósito</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0">
+              <a:latin typeface="Open sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Open sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Open sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> de este archivo excel es poder tener mejor seguimiento de las incidencias épicas que estarán en JIRA. Ya que la interfaz no separá las épicas por usuario.</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES" sz="1100">
+            <a:latin typeface="Open sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Open sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Open sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{858EA32D-F0CB-4A76-985C-56C12EC9869D}" name="Tabla2" displayName="Tabla2" ref="B8:C24" totalsRowCount="1" headerRowDxfId="14" dataDxfId="15">
+  <autoFilter ref="B8:C23" xr:uid="{858EA32D-F0CB-4A76-985C-56C12EC9869D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{84E63D7B-3CB8-4C9F-9FD3-66FB6068667C}" name="Epica" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{16CF8D34-B4E1-4F29-BD5C-6918DE397E47}" name="Cantidad de HU" totalsRowFunction="count" dataDxfId="16" totalsRowDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{172A9739-957D-442D-A067-2612ACD67246}" name="Tabla3" displayName="Tabla3" ref="D8:E24" totalsRowCount="1" headerRowDxfId="10" dataDxfId="11">
+  <autoFilter ref="D8:E23" xr:uid="{172A9739-957D-442D-A067-2612ACD67246}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{76CA7D33-2043-43EA-B790-BC9475198FC9}" name="Epica" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{BB9D40FF-329E-49FA-9D1F-36E33960214D}" name="Cantidad de HU" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{634ED8CA-E6D1-4309-AC04-2AFB015BD731}" name="Tabla4" displayName="Tabla4" ref="F8:G24" totalsRowCount="1" headerRowDxfId="6" dataDxfId="7">
+  <autoFilter ref="F8:G23" xr:uid="{634ED8CA-E6D1-4309-AC04-2AFB015BD731}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{19EB42D7-85B5-4FA0-9A07-EC583BD5E82B}" name="Epica" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{17AF23ED-6EBB-4BCA-BB2D-FE6F09145C3C}" name="Cantidad de HU" totalsRowFunction="count" dataDxfId="8" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +861,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A5:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="40.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="40.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2">
+        <f>SUBTOTAL(103,Tabla2[Cantidad de HU])</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2">
+        <f>SUBTOTAL(103,Tabla3[Cantidad de HU])</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="2">
+        <f>SUBTOTAL(103,Tabla4[Cantidad de HU])</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="B7:C7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="3">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>